<commit_message>
passage de la quantité de int à float : Modif des changeTable Modif des jframe
</commit_message>
<xml_diff>
--- a/BonDeCommande/bonDeCommandeTest.xlsx
+++ b/BonDeCommande/bonDeCommandeTest.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="42">
   <si>
     <t xml:space="preserve">DESIGNATION </t>
   </si>
@@ -113,43 +113,40 @@
     <t>x</t>
   </si>
   <si>
-    <t>Montant total HT :  0.0 €</t>
+    <t>Montant total HT :  158.5 €</t>
   </si>
   <si>
     <t xml:space="preserve">LIEU DE LIVRAISON :   - </t>
   </si>
   <si>
-    <t>DATE DE LIVRAISON SOUHAITEE :  mardi 16 octobre 2018 - POMPE : 08h00</t>
-  </si>
-  <si>
-    <t>Flèche 24 ou 28 ml ou plus</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>ml</t>
-  </si>
-  <si>
-    <t>0.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Centrale : </t>
+    <t xml:space="preserve">DATE DE LIVRAISON SOUHAITEE :  </t>
+  </si>
+  <si>
+    <t>BPS C25/30 XF1 320 KG</t>
+  </si>
+  <si>
+    <t>5.63</t>
+  </si>
+  <si>
+    <t>m³</t>
+  </si>
+  <si>
+    <t>31.7</t>
+  </si>
+  <si>
+    <t>+COMPLÉMENT</t>
   </si>
   <si>
     <t/>
   </si>
   <si>
-    <t xml:space="preserve">Tel : </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Heure pompe : </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Heure béton : </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Volume : </t>
+    <t>COULAGE À LA POMPE FOURNIE PAR SOL2S</t>
+  </si>
+  <si>
+    <t>COULAGE À LA POMPE FOURNIE PAR VOS SOINS</t>
+  </si>
+  <si>
+    <t>BPS C25/30 XF1 320KG CPJ42.5 S4 D.MAX 22.4 CL 0.40</t>
   </si>
 </sst>
 </file>
@@ -1348,14 +1345,14 @@
         <v>35</v>
       </c>
       <c r="D15" s="17" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E15" s="17" t="s">
         <v>36</v>
       </c>
     </row>
     <row customHeight="1" ht="25.5" r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="17" t="s">
+      <c r="A16" s="35" t="s">
         <v>37</v>
       </c>
       <c r="B16" s="17" t="s">
@@ -1365,14 +1362,14 @@
         <v>38</v>
       </c>
       <c r="D16" s="17" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E16" s="17" t="s">
         <v>36</v>
       </c>
     </row>
     <row customHeight="1" ht="25.5" r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="17" t="s">
+      <c r="A17" s="35" t="s">
         <v>39</v>
       </c>
       <c r="B17" s="17" t="s">
@@ -1382,14 +1379,14 @@
         <v>38</v>
       </c>
       <c r="D17" s="17" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E17" s="17" t="s">
         <v>36</v>
       </c>
     </row>
     <row customHeight="1" ht="25.5" r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="17" t="s">
+      <c r="A18" s="35" t="s">
         <v>40</v>
       </c>
       <c r="B18" s="17" t="s">
@@ -1399,7 +1396,7 @@
         <v>38</v>
       </c>
       <c r="D18" s="17" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E18" s="17" t="s">
         <v>36</v>
@@ -1416,28 +1413,18 @@
         <v>38</v>
       </c>
       <c r="D19" s="17" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E19" s="17" t="s">
         <v>36</v>
       </c>
     </row>
     <row customHeight="1" ht="25.5" r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="B20" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="C20" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="D20" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="E20" s="17" t="s">
-        <v>36</v>
-      </c>
+      <c r="A20" s="17"/>
+      <c r="B20" s="17"/>
+      <c r="C20" s="17"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="17"/>
     </row>
     <row customHeight="1" ht="25.5" r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="17"/>

</xml_diff>